<commit_message>
atualização da página e menus para relatórios
</commit_message>
<xml_diff>
--- a/_data/in_xls/contagens_orientacoes.xlsx
+++ b/_data/in_xls/contagens_orientacoes.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -517,14 +517,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>em andamento</t>
+          <t>concluídas</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -535,14 +535,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>concluídas</t>
+          <t>em andamento</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -607,14 +607,14 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>concluídas</t>
+          <t>em andamento</t>
         </is>
       </c>
       <c r="C10" t="n">
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
@@ -625,14 +625,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>em andamento</t>
+          <t>concluídas</t>
         </is>
       </c>
       <c r="C11" t="n">
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -895,14 +895,14 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>em andamento</t>
+          <t>concluídas</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27">
@@ -913,14 +913,14 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>concluídas</t>
+          <t>em andamento</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D27" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28">
@@ -985,14 +985,14 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>concluídas</t>
+          <t>em andamento</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1003,14 +1003,14 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>em andamento</t>
+          <t>concluídas</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
@@ -1057,11 +1057,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>em andamento</t>
+          <t>concluídas</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D35" t="n">
         <v>0</v>
@@ -1075,11 +1075,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>concluídas</t>
+          <t>em andamento</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D36" t="n">
         <v>0</v>
@@ -1129,14 +1129,14 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>em andamento</t>
+          <t>concluídas</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D39" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40">
@@ -1147,14 +1147,14 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>concluídas</t>
+          <t>em andamento</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D40" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -1165,14 +1165,14 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>em andamento</t>
+          <t>concluídas</t>
         </is>
       </c>
       <c r="C41" t="n">
+        <v>8</v>
+      </c>
+      <c r="D41" t="n">
         <v>3</v>
-      </c>
-      <c r="D41" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1183,14 +1183,14 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>concluídas</t>
+          <t>em andamento</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D42" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">

</xml_diff>

<commit_message>
atualização de extração para outubro
</commit_message>
<xml_diff>
--- a/_data/in_xls/contagens_orientacoes.xlsx
+++ b/_data/in_xls/contagens_orientacoes.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,14 +517,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>concluídas</t>
+          <t>em andamento</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -535,14 +535,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>em andamento</t>
+          <t>concluídas</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -607,14 +607,14 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>em andamento</t>
+          <t>concluídas</t>
         </is>
       </c>
       <c r="C10" t="n">
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -625,14 +625,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>concluídas</t>
+          <t>em andamento</t>
         </is>
       </c>
       <c r="C11" t="n">
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
@@ -710,7 +710,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Gilvan Pessoa Furtado</t>
+          <t>Galba Freire Moita</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -722,7 +722,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -733,32 +733,32 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>em andamento</t>
+          <t>concluídas</t>
         </is>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Giovanny Augusto Camacho Antevere Mazzarotto</t>
+          <t>Gilvan Pessoa Furtado</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>concluídas</t>
+          <t>em andamento</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -782,7 +782,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Ivana Cristina de Holanda Cunha Barreto</t>
+          <t>Giovanny Augusto Camacho Antevere Mazzarotto</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -791,10 +791,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D20" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -805,20 +805,20 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>em andamento</t>
+          <t>concluídas</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D21" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Jaime Ribeiro Filho</t>
+          <t>Ivana Cristina de Holanda Cunha Barreto</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -827,10 +827,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23">
@@ -841,20 +841,20 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>concluídas</t>
+          <t>em andamento</t>
         </is>
       </c>
       <c r="C23" t="n">
         <v>2</v>
       </c>
       <c r="D23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>João Hermínio Martins da Silva</t>
+          <t>Jaime Ribeiro Filho</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -863,10 +863,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D24" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -877,32 +877,32 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>em andamento</t>
+          <t>concluídas</t>
         </is>
       </c>
       <c r="C25" t="n">
         <v>5</v>
       </c>
       <c r="D25" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Luiz Odorico Monteiro de Andrade</t>
+          <t>João Hermínio Martins da Silva</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>concluídas</t>
+          <t>em andamento</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D26" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
@@ -926,7 +926,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Marcela Helena Gambim Fonseca</t>
+          <t>Luiz Odorico Monteiro de Andrade</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -935,16 +935,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D28" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Marcos Roberto Lourenzoni</t>
+          <t>Marcela Helena Gambim Fonseca</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -953,10 +953,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
@@ -980,19 +980,19 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Maximiliano Ponte</t>
+          <t>Marcos Roberto Lourenzoni</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>em andamento</t>
+          <t>concluídas</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32">
@@ -1016,7 +1016,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Márcio Flávio Moura de Araújo</t>
+          <t>Maximiliano Ponte</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1025,10 +1025,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1039,20 +1039,20 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>concluídas</t>
+          <t>em andamento</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D34" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Regis Bernardo Brandim Gomes</t>
+          <t>Márcio Flávio Moura de Araújo</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1061,10 +1061,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36">
@@ -1088,7 +1088,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Roberto Nicolete</t>
+          <t>Regis Bernardo Brandim Gomes</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1097,10 +1097,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D37" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1111,32 +1111,32 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>em andamento</t>
+          <t>concluídas</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Roberto Wagner Júnior Freire de Freitas</t>
+          <t>Roberto Nicolete</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>concluídas</t>
+          <t>em andamento</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40">
@@ -1160,7 +1160,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Sharmênia de Araújo Soares Nuto</t>
+          <t>Roberto Wagner Júnior Freire de Freitas</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1169,10 +1169,10 @@
         </is>
       </c>
       <c r="C41" t="n">
+        <v>7</v>
+      </c>
+      <c r="D41" t="n">
         <v>8</v>
-      </c>
-      <c r="D41" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="42">
@@ -1183,32 +1183,32 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>em andamento</t>
+          <t>concluídas</t>
         </is>
       </c>
       <c r="C42" t="n">
+        <v>8</v>
+      </c>
+      <c r="D42" t="n">
         <v>3</v>
-      </c>
-      <c r="D42" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Vanira Matos Pessoa</t>
+          <t>Sharmênia de Araújo Soares Nuto</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>concluídas</t>
+          <t>em andamento</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1219,13 +1219,31 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>em andamento</t>
+          <t>concluídas</t>
         </is>
       </c>
       <c r="C44" t="n">
+        <v>12</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Vanira Matos Pessoa</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>em andamento</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
         <v>7</v>
       </c>
-      <c r="D44" t="n">
+      <c r="D45" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>